<commit_message>
Update PRC_ISA exception tables UI Requirements.xlsx
</commit_message>
<xml_diff>
--- a/PRC_ISA exception tables UI Requirements.xlsx
+++ b/PRC_ISA exception tables UI Requirements.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Projects\Item Sub Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eah07vx\Documents\GitHub\pal-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E4BEEE-E61A-4A14-B8E9-C77B1BE72D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="330" windowWidth="6480" windowHeight="3570"/>
+    <workbookView xWindow="37110" yWindow="4170" windowWidth="22320" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="4" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>ISA exception table:  01 Formulary item</t>
   </si>
@@ -183,12 +184,15 @@
   </si>
   <si>
     <t>Cloud AWS or Azure with table set up in HANA</t>
+  </si>
+  <si>
+    <t>Make a change to demo github descktop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
@@ -830,29 +834,29 @@
   </cellXfs>
   <cellStyles count="60">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="47"/>
+    <cellStyle name="20% - Accent1 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="49"/>
+    <cellStyle name="20% - Accent2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="51"/>
+    <cellStyle name="20% - Accent3 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="53"/>
+    <cellStyle name="20% - Accent4 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="55"/>
+    <cellStyle name="20% - Accent5 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="57"/>
+    <cellStyle name="20% - Accent6 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="48"/>
+    <cellStyle name="40% - Accent1 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="50"/>
+    <cellStyle name="40% - Accent2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="52"/>
+    <cellStyle name="40% - Accent3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="54"/>
+    <cellStyle name="40% - Accent4 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="56"/>
+    <cellStyle name="40% - Accent5 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="58"/>
+    <cellStyle name="40% - Accent6 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
@@ -878,14 +882,14 @@
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="45"/>
-    <cellStyle name="Normal 3" xfId="43"/>
-    <cellStyle name="Normal 4" xfId="44"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 3" xfId="43" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 4" xfId="44" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
     <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="46"/>
+    <cellStyle name="Note 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="SAPBEXstdItem 2" xfId="59"/>
+    <cellStyle name="SAPBEXstdItem 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
@@ -915,7 +919,13 @@
     <xdr:ext cx="7848600" cy="2205989"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1067,7 +1077,13 @@
     <xdr:ext cx="7839075" cy="5353004"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1746,11 +1762,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A46:C64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,6 +1776,11 @@
     <col min="3" max="3" width="79.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>23</v>
@@ -1866,7 +1887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -2209,7 +2230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2515,7 +2536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>